<commit_message>
Update edited session - 2025-12-05T12:45:00.098Z - Cache Bust ID: 1764938700099ayzb3wcwp
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Physiology_scanner1764839842978_64d00f214e61c80b5da85b6c2a6d069e7300641b5deff43e650562df72e017a9.xlsx
+++ b/log_history/Y2_B2526_Physiology_scanner1764839842978_64d00f214e61c80b5da85b6c2a6d069e7300641b5deff43e650562df72e017a9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>244484</v>
+        <v>244573</v>
       </c>
       <c r="B33" t="str">
         <v>Physiology</v>
@@ -1053,7 +1053,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:18:36</v>
+        <v>11:18:40</v>
       </c>
       <c r="E33" t="str">
         <v>Scan</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>244573</v>
+        <v>244630</v>
       </c>
       <c r="B34" t="str">
         <v>Physiology</v>
@@ -1073,7 +1073,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:18:40</v>
+        <v>11:18:43</v>
       </c>
       <c r="E34" t="str">
         <v>Scan</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>244630</v>
+        <v>244639</v>
       </c>
       <c r="B35" t="str">
         <v>Physiology</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>244639</v>
+        <v>244479</v>
       </c>
       <c r="B36" t="str">
         <v>Physiology</v>
@@ -1113,7 +1113,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:18:43</v>
+        <v>11:18:44</v>
       </c>
       <c r="E36" t="str">
         <v>Scan</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>244479</v>
+        <v>244605</v>
       </c>
       <c r="B37" t="str">
         <v>Physiology</v>
@@ -1133,7 +1133,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:18:44</v>
+        <v>11:18:50</v>
       </c>
       <c r="E37" t="str">
         <v>Scan</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>244605</v>
+        <v>244582</v>
       </c>
       <c r="B38" t="str">
         <v>Physiology</v>
@@ -1153,7 +1153,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:18:50</v>
+        <v>11:18:54</v>
       </c>
       <c r="E38" t="str">
         <v>Scan</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>244582</v>
+        <v>244627</v>
       </c>
       <c r="B39" t="str">
         <v>Physiology</v>
@@ -1173,7 +1173,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:18:54</v>
+        <v>11:18:56</v>
       </c>
       <c r="E39" t="str">
         <v>Scan</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>244627</v>
+        <v>244625</v>
       </c>
       <c r="B40" t="str">
         <v>Physiology</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>244625</v>
+        <v>244480</v>
       </c>
       <c r="B41" t="str">
         <v>Physiology</v>
@@ -1213,7 +1213,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:18:56</v>
+        <v>11:19:03</v>
       </c>
       <c r="E41" t="str">
         <v>Scan</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>244480</v>
+        <v>244478</v>
       </c>
       <c r="B42" t="str">
         <v>Physiology</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>244478</v>
+        <v>244570</v>
       </c>
       <c r="B43" t="str">
         <v>Physiology</v>
@@ -1253,10 +1253,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:19:03</v>
+        <v>11:19:16</v>
       </c>
       <c r="E43" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F43" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>244570</v>
+        <v>244610</v>
       </c>
       <c r="B44" t="str">
         <v>Physiology</v>
@@ -1273,7 +1273,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:19:16</v>
+        <v>11:19:24</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>244610</v>
+        <v>244581</v>
       </c>
       <c r="B45" t="str">
         <v>Physiology</v>
@@ -1293,7 +1293,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:19:24</v>
+        <v>11:19:32</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>244581</v>
+        <v>244587</v>
       </c>
       <c r="B46" t="str">
         <v>Physiology</v>
@@ -1313,10 +1313,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:19:32</v>
+        <v>11:19:34</v>
       </c>
       <c r="E46" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F46" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>244587</v>
+        <v>244574</v>
       </c>
       <c r="B47" t="str">
         <v>Physiology</v>
@@ -1333,10 +1333,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:19:34</v>
+        <v>11:19:41</v>
       </c>
       <c r="E47" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F47" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>244574</v>
+        <v>244635</v>
       </c>
       <c r="B48" t="str">
         <v>Physiology</v>
@@ -1353,10 +1353,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:19:41</v>
+        <v>11:19:58</v>
       </c>
       <c r="E48" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F48" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>244635</v>
+        <v>244588</v>
       </c>
       <c r="B49" t="str">
         <v>Physiology</v>
@@ -1373,10 +1373,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:19:58</v>
+        <v>11:20:12</v>
       </c>
       <c r="E49" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F49" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>244588</v>
+        <v>244469</v>
       </c>
       <c r="B50" t="str">
         <v>Physiology</v>
@@ -1393,10 +1393,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:20:12</v>
+        <v>11:21:31</v>
       </c>
       <c r="E50" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F50" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>244469</v>
+        <v>244593</v>
       </c>
       <c r="B51" t="str">
         <v>Physiology</v>
@@ -1413,7 +1413,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:21:31</v>
+        <v>11:21:35</v>
       </c>
       <c r="E51" t="str">
         <v>Scan</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>244593</v>
+        <v>244637</v>
       </c>
       <c r="B52" t="str">
         <v>Physiology</v>
@@ -1433,7 +1433,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:21:35</v>
+        <v>11:21:37</v>
       </c>
       <c r="E52" t="str">
         <v>Scan</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>244637</v>
+        <v>244572</v>
       </c>
       <c r="B53" t="str">
         <v>Physiology</v>
@@ -1453,7 +1453,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:21:37</v>
+        <v>11:22:00</v>
       </c>
       <c r="E53" t="str">
         <v>Scan</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>244572</v>
+        <v>244583</v>
       </c>
       <c r="B54" t="str">
         <v>Physiology</v>
@@ -1473,7 +1473,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:22:00</v>
+        <v>11:22:03</v>
       </c>
       <c r="E54" t="str">
         <v>Scan</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>244583</v>
+        <v>244568</v>
       </c>
       <c r="B55" t="str">
         <v>Physiology</v>
@@ -1493,7 +1493,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:22:03</v>
+        <v>11:22:18</v>
       </c>
       <c r="E55" t="str">
         <v>Scan</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>244568</v>
+        <v>244595</v>
       </c>
       <c r="B56" t="str">
         <v>Physiology</v>
@@ -1513,10 +1513,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:22:18</v>
+        <v>11:23:13</v>
       </c>
       <c r="E56" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F56" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>244595</v>
+        <v>244467</v>
       </c>
       <c r="B57" t="str">
         <v>Physiology</v>
@@ -1533,10 +1533,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:23:13</v>
+        <v>11:39:48</v>
       </c>
       <c r="E57" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F57" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>244467</v>
+        <v>244466</v>
       </c>
       <c r="B58" t="str">
         <v>Physiology</v>
@@ -1553,7 +1553,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:39:48</v>
+        <v>11:39:49</v>
       </c>
       <c r="E58" t="str">
         <v>Scan</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>244466</v>
+        <v>244456</v>
       </c>
       <c r="B59" t="str">
         <v>Physiology</v>
@@ -1573,7 +1573,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:39:49</v>
+        <v>11:40:02</v>
       </c>
       <c r="E59" t="str">
         <v>Scan</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>244456</v>
+        <v>244472</v>
       </c>
       <c r="B60" t="str">
         <v>Physiology</v>
@@ -1593,7 +1593,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:40:02</v>
+        <v>11:40:08</v>
       </c>
       <c r="E60" t="str">
         <v>Scan</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>244472</v>
+        <v>244455</v>
       </c>
       <c r="B61" t="str">
         <v>Physiology</v>
@@ -1613,7 +1613,7 @@
         <v>04/12/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:40:08</v>
+        <v>11:40:29</v>
       </c>
       <c r="E61" t="str">
         <v>Scan</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>244455</v>
+        <v>244470</v>
       </c>
       <c r="B62" t="str">
         <v>Physiology</v>
@@ -1633,10 +1633,10 @@
         <v>04/12/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:40:29</v>
+        <v>11:41:02</v>
       </c>
       <c r="E62" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F62" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>244470</v>
+        <v>244571</v>
       </c>
       <c r="B63" t="str">
         <v>Physiology</v>
@@ -1653,38 +1653,18 @@
         <v>04/12/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:41:02</v>
+        <v>11:41:50</v>
       </c>
       <c r="E63" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F63" t="str">
-        <v>wafaa.ebida@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>244571</v>
-      </c>
-      <c r="B64" t="str">
-        <v>Physiology</v>
-      </c>
-      <c r="C64" t="str">
-        <v>04/12/2025</v>
-      </c>
-      <c r="D64" t="str">
-        <v>11:41:50</v>
-      </c>
-      <c r="E64" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F64" t="str">
         <v>wafaa.ebida@med.asu.edu.eg</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F64"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F63"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>